<commit_message>
Added in direction of entry for each room.
</commit_message>
<xml_diff>
--- a/Maps/E5/Directory/e5.xlsx
+++ b/Maps/E5/Directory/e5.xlsx
@@ -21,6 +21,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="4">
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,15 +353,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3034</v>
       </c>
@@ -354,8 +371,11 @@
       <c r="C1">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3036</v>
       </c>
@@ -365,8 +385,11 @@
       <c r="C2">
         <v>137</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3037</v>
       </c>
@@ -376,8 +399,11 @@
       <c r="C3">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3906</v>
       </c>
@@ -387,8 +413,11 @@
       <c r="C4">
         <v>137</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3042</v>
       </c>
@@ -398,8 +427,11 @@
       <c r="C5">
         <v>137</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3043</v>
       </c>
@@ -409,8 +441,11 @@
       <c r="C6">
         <v>137</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3046</v>
       </c>
@@ -420,8 +455,11 @@
       <c r="C7">
         <v>137</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3047</v>
       </c>
@@ -431,8 +469,11 @@
       <c r="C8">
         <v>137</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3048</v>
       </c>
@@ -442,8 +483,11 @@
       <c r="C9">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3051</v>
       </c>
@@ -453,8 +497,11 @@
       <c r="C10">
         <v>137</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3054</v>
       </c>
@@ -464,8 +511,11 @@
       <c r="C11">
         <v>137</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3053</v>
       </c>
@@ -475,8 +525,11 @@
       <c r="C12">
         <v>137</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3106</v>
       </c>
@@ -486,8 +539,11 @@
       <c r="C13">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3107</v>
       </c>
@@ -497,8 +553,11 @@
       <c r="C14">
         <v>137</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3108</v>
       </c>
@@ -508,8 +567,11 @@
       <c r="C15">
         <v>137</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3109</v>
       </c>
@@ -519,8 +581,11 @@
       <c r="C16">
         <v>137</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3133</v>
       </c>
@@ -530,8 +595,11 @@
       <c r="C17">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3904</v>
       </c>
@@ -541,8 +609,11 @@
       <c r="C18">
         <v>137</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3111</v>
       </c>
@@ -552,8 +623,11 @@
       <c r="C19">
         <v>163</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3807</v>
       </c>
@@ -563,8 +637,11 @@
       <c r="C20">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3804</v>
       </c>
@@ -574,8 +651,11 @@
       <c r="C21">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3806</v>
       </c>
@@ -585,8 +665,11 @@
       <c r="C22">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3027</v>
       </c>
@@ -596,8 +679,11 @@
       <c r="C23">
         <v>630</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3026</v>
       </c>
@@ -607,8 +693,11 @@
       <c r="C24">
         <v>630</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3024</v>
       </c>
@@ -618,8 +707,11 @@
       <c r="C25">
         <v>630</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3023</v>
       </c>
@@ -629,8 +721,11 @@
       <c r="C26">
         <v>630</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3022</v>
       </c>
@@ -640,8 +735,11 @@
       <c r="C27">
         <v>630</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3017</v>
       </c>
@@ -651,8 +749,11 @@
       <c r="C28">
         <v>630</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3016</v>
       </c>
@@ -662,8 +763,11 @@
       <c r="C29">
         <v>630</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3013</v>
       </c>
@@ -673,8 +777,11 @@
       <c r="C30">
         <v>630</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3011</v>
       </c>
@@ -684,8 +791,11 @@
       <c r="C31">
         <v>630</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3009</v>
       </c>
@@ -695,8 +805,11 @@
       <c r="C32">
         <v>630</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3007</v>
       </c>
@@ -706,8 +819,11 @@
       <c r="C33">
         <v>630</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3004</v>
       </c>
@@ -717,8 +833,11 @@
       <c r="C34">
         <v>630</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3003</v>
       </c>
@@ -728,8 +847,11 @@
       <c r="C35">
         <v>630</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3002</v>
       </c>
@@ -739,8 +861,11 @@
       <c r="C36">
         <v>630</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3033</v>
       </c>
@@ -750,8 +875,11 @@
       <c r="C37">
         <v>218</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3032</v>
       </c>
@@ -761,8 +889,11 @@
       <c r="C38">
         <v>303</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3031</v>
       </c>
@@ -772,8 +903,11 @@
       <c r="C39">
         <v>465</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3029</v>
       </c>
@@ -783,8 +917,11 @@
       <c r="C40">
         <v>550</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3038</v>
       </c>
@@ -794,8 +931,11 @@
       <c r="C41">
         <v>192</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3039</v>
       </c>
@@ -805,8 +945,11 @@
       <c r="C42">
         <v>192</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3020</v>
       </c>
@@ -816,8 +959,11 @@
       <c r="C43">
         <v>434</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3019</v>
       </c>
@@ -827,8 +973,11 @@
       <c r="C44">
         <v>482</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3041</v>
       </c>
@@ -838,8 +987,11 @@
       <c r="C45">
         <v>192</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3044</v>
       </c>
@@ -849,8 +1001,11 @@
       <c r="C46">
         <v>192</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3018</v>
       </c>
@@ -860,8 +1015,11 @@
       <c r="C47">
         <v>577</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3014</v>
       </c>
@@ -871,8 +1029,11 @@
       <c r="C48">
         <v>577</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3008</v>
       </c>
@@ -882,8 +1043,11 @@
       <c r="C49">
         <v>577</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3012</v>
       </c>
@@ -893,8 +1057,11 @@
       <c r="C50">
         <v>577</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3049</v>
       </c>
@@ -904,8 +1071,11 @@
       <c r="C51">
         <v>192</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3052</v>
       </c>
@@ -915,8 +1085,11 @@
       <c r="C52">
         <v>192</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3006</v>
       </c>
@@ -926,8 +1099,11 @@
       <c r="C53">
         <v>577</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3001</v>
       </c>
@@ -937,8 +1113,11 @@
       <c r="C54">
         <v>577</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3801</v>
       </c>
@@ -948,8 +1127,11 @@
       <c r="C55">
         <v>241</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3802</v>
       </c>
@@ -959,8 +1141,11 @@
       <c r="C56">
         <v>326</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3901</v>
       </c>
@@ -970,8 +1155,11 @@
       <c r="C57">
         <v>395</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3902</v>
       </c>
@@ -981,8 +1169,11 @@
       <c r="C58">
         <v>458</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3803</v>
       </c>
@@ -992,8 +1183,11 @@
       <c r="C59">
         <v>575</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3903</v>
       </c>
@@ -1002,6 +1196,9 @@
       </c>
       <c r="C60">
         <v>193</v>
+      </c>
+      <c r="D60" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>